<commit_message>
fix cisa vendor assessment
</commit_message>
<xml_diff>
--- a/tools/cisa/cisa-vendor-scrm.xlsx
+++ b/tools/cisa/cisa-vendor-scrm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/cisa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BD314F-4D2A-BD45-A767-E42BDC8F58EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F64490-8850-F144-8B1E-EF380AD66473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" activeTab="1" xr2:uid="{7CC275B4-B827-4C40-A91C-0378AFDDCA47}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="590">
   <si>
     <t>id</t>
   </si>
@@ -2404,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DB2561-4FB2-3748-AEC3-1AEA98CB57DC}">
   <dimension ref="A1:H287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" zoomScale="133" workbookViewId="0">
-      <selection activeCell="C271" sqref="C271:C287"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2444,6 +2444,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>

</xml_diff>